<commit_message>
Fixed mistake in BOM
</commit_message>
<xml_diff>
--- a/Algemeen/Bestellijst.xlsx
+++ b/Algemeen/Bestellijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick\Documents\GitHub\Plan-T\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E54EC5-F30E-46F6-9687-B365AB3D7CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E0E1685-48A2-424A-B70D-921B8C1909BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{6E9411CA-CAA6-4A90-993D-0569070D53C6}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="353">
   <si>
     <t>Component</t>
   </si>
@@ -230,9 +230,6 @@
     <t>PH- sensor + ADC</t>
   </si>
   <si>
-    <t>UV-C filter (nieuw)</t>
-  </si>
-  <si>
     <t>Componenten PCB</t>
   </si>
   <si>
@@ -1104,6 +1101,12 @@
   </si>
   <si>
     <t>gerecupereerd</t>
+  </si>
+  <si>
+    <t>yyyyy</t>
+  </si>
+  <si>
+    <t>UV-C filter (nieuw) [14W - ordinary]</t>
   </si>
 </sst>
 </file>
@@ -1841,7 +1844,7 @@
   <dimension ref="A1:P214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2800,7 +2803,7 @@
     </row>
     <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
-        <v>60</v>
+        <v>352</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>16</v>
@@ -2828,35 +2831,35 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="C28" s="41" t="s">
         <v>63</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>64</v>
       </c>
       <c r="I28"/>
       <c r="J28"/>
       <c r="L28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>67</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29">
@@ -2872,24 +2875,24 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>71</v>
-      </c>
-      <c r="C30" t="s">
-        <v>72</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30">
@@ -2905,24 +2908,24 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>74</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31">
@@ -2938,31 +2941,31 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
         <v>75</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>76</v>
-      </c>
-      <c r="C32" t="s">
-        <v>77</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32">
-        <v>1</v>
+      <c r="F32" t="s">
+        <v>351</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -2971,24 +2974,24 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
         <v>78</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>79</v>
-      </c>
-      <c r="C33" t="s">
-        <v>80</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33">
@@ -3004,24 +3007,24 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
         <v>81</v>
-      </c>
-      <c r="C34" t="s">
-        <v>82</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34">
@@ -3037,24 +3040,24 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" t="s">
         <v>83</v>
-      </c>
-      <c r="C35" t="s">
-        <v>84</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35">
@@ -3070,24 +3073,24 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
         <v>85</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>86</v>
-      </c>
-      <c r="C36" t="s">
-        <v>87</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36">
@@ -3103,24 +3106,24 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" t="s">
         <v>88</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>89</v>
-      </c>
-      <c r="C37" t="s">
-        <v>90</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37">
@@ -3136,24 +3139,24 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" t="s">
         <v>91</v>
-      </c>
-      <c r="C38" t="s">
-        <v>92</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38">
@@ -3169,24 +3172,24 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
         <v>93</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>94</v>
-      </c>
-      <c r="C39" t="s">
-        <v>95</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39">
@@ -3202,24 +3205,24 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
         <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" t="s">
-        <v>97</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40">
@@ -3235,24 +3238,24 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
         <v>98</v>
-      </c>
-      <c r="B41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" t="s">
-        <v>99</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41">
@@ -3268,24 +3271,24 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" t="s">
         <v>100</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>101</v>
-      </c>
-      <c r="C42" t="s">
-        <v>102</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42">
@@ -3301,24 +3304,24 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" t="s">
         <v>103</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>104</v>
-      </c>
-      <c r="C43" t="s">
-        <v>105</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43">
@@ -3334,24 +3337,24 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
         <v>106</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>107</v>
-      </c>
-      <c r="C44" t="s">
-        <v>108</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44">
@@ -3367,24 +3370,24 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
         <v>109</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>110</v>
-      </c>
-      <c r="C45" t="s">
-        <v>111</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45">
@@ -3400,24 +3403,24 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
         <v>112</v>
-      </c>
-      <c r="C46" t="s">
-        <v>113</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46">
@@ -3433,24 +3436,24 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
         <v>114</v>
-      </c>
-      <c r="B47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" t="s">
-        <v>115</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47">
@@ -3466,24 +3469,24 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" t="s">
         <v>116</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>117</v>
-      </c>
-      <c r="C48" t="s">
-        <v>118</v>
       </c>
       <c r="D48" s="10"/>
       <c r="E48">
@@ -3499,24 +3502,24 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" t="s">
         <v>119</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>120</v>
-      </c>
-      <c r="C49" t="s">
-        <v>121</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49">
@@ -3532,24 +3535,24 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" t="s">
         <v>122</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>123</v>
-      </c>
-      <c r="C50" t="s">
-        <v>124</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50">
@@ -3565,24 +3568,24 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
         <v>125</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>126</v>
-      </c>
-      <c r="C51" t="s">
-        <v>127</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51">
@@ -3598,24 +3601,24 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" t="s">
         <v>128</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>129</v>
-      </c>
-      <c r="C52" t="s">
-        <v>130</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52">
@@ -3631,24 +3634,24 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" t="s">
         <v>131</v>
-      </c>
-      <c r="C53" t="s">
-        <v>132</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53">
@@ -3664,24 +3667,24 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" t="s">
         <v>133</v>
-      </c>
-      <c r="C54" t="s">
-        <v>134</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54">
@@ -3697,24 +3700,24 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" t="s">
         <v>135</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>136</v>
-      </c>
-      <c r="C55" t="s">
-        <v>137</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55">
@@ -3730,24 +3733,24 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" t="s">
         <v>138</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>139</v>
-      </c>
-      <c r="C56" t="s">
-        <v>140</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56">
@@ -3763,24 +3766,24 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" t="s">
         <v>141</v>
-      </c>
-      <c r="C57" t="s">
-        <v>142</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57">
@@ -3796,24 +3799,24 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58" t="s">
         <v>143</v>
-      </c>
-      <c r="C58" t="s">
-        <v>144</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58">
@@ -3829,24 +3832,24 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" t="s">
         <v>145</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>146</v>
-      </c>
-      <c r="C59" t="s">
-        <v>147</v>
       </c>
       <c r="D59" s="10"/>
       <c r="E59">
@@ -3862,24 +3865,24 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B60" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" t="s">
         <v>148</v>
-      </c>
-      <c r="C60" t="s">
-        <v>149</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60">
@@ -3895,24 +3898,24 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" t="s">
         <v>150</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>151</v>
-      </c>
-      <c r="C61" t="s">
-        <v>152</v>
       </c>
       <c r="D61" s="10"/>
       <c r="E61">
@@ -3928,24 +3931,24 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B62" t="s">
+        <v>152</v>
+      </c>
+      <c r="C62" t="s">
         <v>153</v>
-      </c>
-      <c r="C62" t="s">
-        <v>154</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62">
@@ -3961,24 +3964,24 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" t="s">
         <v>155</v>
-      </c>
-      <c r="C63" t="s">
-        <v>156</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63">
@@ -3994,24 +3997,24 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B64" t="s">
+        <v>156</v>
+      </c>
+      <c r="C64" t="s">
         <v>157</v>
-      </c>
-      <c r="C64" t="s">
-        <v>158</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64">
@@ -4027,24 +4030,24 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" t="s">
         <v>159</v>
-      </c>
-      <c r="C65" t="s">
-        <v>160</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65">
@@ -4060,24 +4063,24 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B66" t="s">
+        <v>160</v>
+      </c>
+      <c r="C66" t="s">
         <v>161</v>
-      </c>
-      <c r="C66" t="s">
-        <v>162</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66">
@@ -4093,24 +4096,24 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
+        <v>162</v>
+      </c>
+      <c r="C67" t="s">
         <v>163</v>
-      </c>
-      <c r="C67" t="s">
-        <v>164</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67">
@@ -4126,24 +4129,24 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" t="s">
         <v>165</v>
-      </c>
-      <c r="C68" t="s">
-        <v>166</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68">
@@ -4159,24 +4162,24 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>166</v>
+      </c>
+      <c r="B69" t="s">
         <v>167</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>168</v>
-      </c>
-      <c r="C69" t="s">
-        <v>169</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69">
@@ -4192,24 +4195,24 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B70" t="s">
+        <v>169</v>
+      </c>
+      <c r="C70" t="s">
         <v>170</v>
-      </c>
-      <c r="C70" t="s">
-        <v>171</v>
       </c>
       <c r="D70" s="10"/>
       <c r="E70">
@@ -4225,24 +4228,24 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
         <v>46</v>
       </c>
       <c r="C71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71">
@@ -4258,24 +4261,24 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
+        <v>172</v>
+      </c>
+      <c r="C72" t="s">
         <v>173</v>
-      </c>
-      <c r="C72" t="s">
-        <v>174</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72">
@@ -4291,24 +4294,24 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B73" t="s">
+        <v>174</v>
+      </c>
+      <c r="C73" t="s">
         <v>175</v>
-      </c>
-      <c r="C73" t="s">
-        <v>176</v>
       </c>
       <c r="D73" s="10"/>
       <c r="E73">
@@ -4324,24 +4327,24 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B74" t="s">
+        <v>176</v>
+      </c>
+      <c r="C74" t="s">
         <v>177</v>
-      </c>
-      <c r="C74" t="s">
-        <v>178</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74">
@@ -4357,24 +4360,24 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
         <v>27</v>
       </c>
       <c r="C75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D75" s="10"/>
       <c r="E75">
@@ -4390,18 +4393,18 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -4415,12 +4418,12 @@
       <c r="K77" s="39"/>
       <c r="L77" s="9"/>
       <c r="M77" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>16</v>
@@ -4447,7 +4450,7 @@
     </row>
     <row r="79" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>16</v>
@@ -4470,7 +4473,7 @@
     </row>
     <row r="80" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>16</v>
@@ -4494,7 +4497,7 @@
     </row>
     <row r="81" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>16</v>
@@ -4517,7 +4520,7 @@
     </row>
     <row r="82" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>16</v>
@@ -4545,7 +4548,7 @@
     </row>
     <row r="83" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>16</v>
@@ -4581,7 +4584,7 @@
     </row>
     <row r="84" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>16</v>
@@ -4616,7 +4619,7 @@
     </row>
     <row r="85" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>16</v>
@@ -4627,7 +4630,7 @@
     </row>
     <row r="86" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>16</v>
@@ -4649,13 +4652,13 @@
     </row>
     <row r="87" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -4684,7 +4687,7 @@
     </row>
     <row r="88" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>16</v>
@@ -4717,7 +4720,7 @@
     </row>
     <row r="89" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>16</v>
@@ -4741,13 +4744,13 @@
     </row>
     <row r="90" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G90">
         <v>2</v>
@@ -4768,7 +4771,7 @@
     </row>
     <row r="91" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>16</v>
@@ -4792,12 +4795,12 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="L91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>16</v>
@@ -4821,18 +4824,18 @@
         <v>6.56</v>
       </c>
       <c r="L92" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -4852,13 +4855,13 @@
     </row>
     <row r="94" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -4878,13 +4881,13 @@
     </row>
     <row r="95" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G95">
         <v>3</v>
@@ -4905,13 +4908,13 @@
     </row>
     <row r="96" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G96">
         <v>2</v>
@@ -4931,13 +4934,13 @@
     </row>
     <row r="97" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C97" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G97">
         <v>2</v>
@@ -4957,13 +4960,13 @@
     </row>
     <row r="98" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G98">
         <v>1</v>
@@ -4983,13 +4986,13 @@
     </row>
     <row r="99" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G99">
         <v>9</v>
@@ -5009,13 +5012,13 @@
     </row>
     <row r="100" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -5035,13 +5038,13 @@
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C101" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -5062,33 +5065,33 @@
     </row>
     <row r="102" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K102" s="2"/>
     </row>
     <row r="103" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B103" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B103" s="60" t="s">
+      <c r="C103" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C103" s="60" t="s">
+      <c r="L103" t="s">
         <v>64</v>
-      </c>
-      <c r="L103" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="57" t="s">
+        <v>213</v>
+      </c>
+      <c r="B104" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C104" s="58" t="s">
         <v>214</v>
-      </c>
-      <c r="B104" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="C104" s="58" t="s">
-        <v>215</v>
       </c>
       <c r="D104">
         <v>5</v>
@@ -5109,13 +5112,13 @@
     </row>
     <row r="105" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B105" s="58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C105" s="58" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D105">
         <v>4</v>
@@ -5136,13 +5139,13 @@
     </row>
     <row r="106" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B106" s="58" t="s">
+        <v>216</v>
+      </c>
+      <c r="C106" s="58" t="s">
         <v>217</v>
-      </c>
-      <c r="C106" s="58" t="s">
-        <v>218</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -5163,13 +5166,13 @@
     </row>
     <row r="107" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B107" s="58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C107" s="58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -5190,13 +5193,13 @@
     </row>
     <row r="108" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="57" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" s="58" t="s">
         <v>220</v>
       </c>
-      <c r="B108" s="58" t="s">
+      <c r="C108" s="58" t="s">
         <v>221</v>
-      </c>
-      <c r="C108" s="58" t="s">
-        <v>222</v>
       </c>
       <c r="D108">
         <v>2</v>
@@ -5217,13 +5220,13 @@
     </row>
     <row r="109" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="B109" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C109" s="58" t="s">
         <v>223</v>
-      </c>
-      <c r="B109" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="C109" s="58" t="s">
-        <v>224</v>
       </c>
       <c r="D109">
         <v>2</v>
@@ -5244,13 +5247,13 @@
     </row>
     <row r="110" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="B110" s="58" t="s">
         <v>225</v>
       </c>
-      <c r="B110" s="58" t="s">
+      <c r="C110" s="58" t="s">
         <v>226</v>
-      </c>
-      <c r="C110" s="58" t="s">
-        <v>227</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -5271,13 +5274,13 @@
     </row>
     <row r="111" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="57" t="s">
+        <v>227</v>
+      </c>
+      <c r="B111" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="B111" s="58" t="s">
+      <c r="C111" s="58" t="s">
         <v>229</v>
-      </c>
-      <c r="C111" s="58" t="s">
-        <v>230</v>
       </c>
       <c r="D111">
         <v>2</v>
@@ -5298,13 +5301,13 @@
     </row>
     <row r="112" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="B112" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="B112" s="58" t="s">
+      <c r="C112" s="58" t="s">
         <v>232</v>
-      </c>
-      <c r="C112" s="58" t="s">
-        <v>233</v>
       </c>
       <c r="D112">
         <v>4</v>
@@ -5325,13 +5328,13 @@
     </row>
     <row r="113" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="B113" s="58" t="s">
         <v>234</v>
       </c>
-      <c r="B113" s="58" t="s">
+      <c r="C113" s="58" t="s">
         <v>235</v>
-      </c>
-      <c r="C113" s="58" t="s">
-        <v>236</v>
       </c>
       <c r="D113">
         <v>2</v>
@@ -5352,13 +5355,13 @@
     </row>
     <row r="114" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="57" t="s">
+        <v>236</v>
+      </c>
+      <c r="B114" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="B114" s="58" t="s">
+      <c r="C114" s="58" t="s">
         <v>238</v>
-      </c>
-      <c r="C114" s="58" t="s">
-        <v>239</v>
       </c>
       <c r="D114">
         <v>2</v>
@@ -5379,13 +5382,13 @@
     </row>
     <row r="115" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="B115" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="B115" s="58" t="s">
+      <c r="C115" s="58" t="s">
         <v>241</v>
-      </c>
-      <c r="C115" s="58" t="s">
-        <v>242</v>
       </c>
       <c r="D115">
         <v>2</v>
@@ -5406,13 +5409,13 @@
     </row>
     <row r="116" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="B116" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="B116" s="58" t="s">
-        <v>244</v>
-      </c>
       <c r="C116" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -5433,13 +5436,13 @@
     </row>
     <row r="117" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="B117" s="58" t="s">
         <v>245</v>
       </c>
-      <c r="B117" s="58" t="s">
-        <v>246</v>
-      </c>
       <c r="C117" s="58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -5460,13 +5463,13 @@
     </row>
     <row r="118" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="B118" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="C118" s="58" t="s">
         <v>247</v>
-      </c>
-      <c r="B118" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="C118" s="58" t="s">
-        <v>248</v>
       </c>
       <c r="D118">
         <v>5</v>
@@ -5487,13 +5490,13 @@
     </row>
     <row r="119" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="B119" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="B119" s="58" t="s">
+      <c r="C119" s="58" t="s">
         <v>250</v>
-      </c>
-      <c r="C119" s="58" t="s">
-        <v>251</v>
       </c>
       <c r="D119">
         <v>4</v>
@@ -5514,13 +5517,13 @@
     </row>
     <row r="120" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B120" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="C120" s="58" t="s">
         <v>252</v>
-      </c>
-      <c r="C120" s="58" t="s">
-        <v>253</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -5541,13 +5544,13 @@
     </row>
     <row r="121" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B121" s="58" t="s">
+        <v>253</v>
+      </c>
+      <c r="C121" s="58" t="s">
         <v>254</v>
-      </c>
-      <c r="C121" s="58" t="s">
-        <v>255</v>
       </c>
       <c r="D121">
         <v>9</v>
@@ -5568,13 +5571,13 @@
     </row>
     <row r="122" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B122" s="58" t="s">
+        <v>255</v>
+      </c>
+      <c r="C122" s="58" t="s">
         <v>256</v>
-      </c>
-      <c r="C122" s="58" t="s">
-        <v>257</v>
       </c>
       <c r="D122">
         <v>3</v>
@@ -5595,13 +5598,13 @@
     </row>
     <row r="123" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="57" t="s">
+        <v>257</v>
+      </c>
+      <c r="B123" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="B123" s="58" t="s">
+      <c r="C123" s="58" t="s">
         <v>259</v>
-      </c>
-      <c r="C123" s="58" t="s">
-        <v>260</v>
       </c>
       <c r="D123">
         <v>2</v>
@@ -5622,13 +5625,13 @@
     </row>
     <row r="124" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="57" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B124" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="C124" s="58" t="s">
         <v>96</v>
-      </c>
-      <c r="C124" s="58" t="s">
-        <v>97</v>
       </c>
       <c r="D124">
         <v>1</v>
@@ -5649,13 +5652,13 @@
     </row>
     <row r="125" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="57" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B125" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C125" s="58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D125">
         <v>1</v>
@@ -5676,13 +5679,13 @@
     </row>
     <row r="126" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="B126" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="B126" s="58" t="s">
-        <v>264</v>
-      </c>
       <c r="C126" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D126">
         <v>1</v>
@@ -5703,10 +5706,10 @@
     </row>
     <row r="128" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="B128" s="22" t="s">
         <v>265</v>
-      </c>
-      <c r="B128" s="22" t="s">
-        <v>266</v>
       </c>
       <c r="C128" s="22"/>
       <c r="D128" s="22"/>
@@ -5719,12 +5722,12 @@
       <c r="K128" s="40"/>
       <c r="L128" s="24"/>
       <c r="M128" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="129" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>16</v>
@@ -5764,7 +5767,7 @@
     </row>
     <row r="130" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>16</v>
@@ -5801,7 +5804,7 @@
     </row>
     <row r="131" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>16</v>
@@ -5838,7 +5841,7 @@
     </row>
     <row r="132" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>16</v>
@@ -5875,7 +5878,7 @@
     </row>
     <row r="133" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>16</v>
@@ -5912,7 +5915,7 @@
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>16</v>
@@ -5949,7 +5952,7 @@
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B135" s="51" t="s">
         <v>16</v>
@@ -5986,7 +5989,7 @@
     </row>
     <row r="136" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B136" s="51" t="s">
         <v>16</v>
@@ -6023,7 +6026,7 @@
     </row>
     <row r="137" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B137" s="51" t="s">
         <v>16</v>
@@ -6048,13 +6051,13 @@
     </row>
     <row r="138" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="58" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B138" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G138">
         <v>1</v>
@@ -6074,12 +6077,12 @@
     </row>
     <row r="140" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="56" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="141" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>16</v>
@@ -6114,18 +6117,18 @@
         <v>4.41</v>
       </c>
       <c r="L141" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="142" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D142">
         <v>20</v>
@@ -6156,13 +6159,13 @@
     </row>
     <row r="143" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D143">
         <v>30</v>
@@ -6193,13 +6196,13 @@
     </row>
     <row r="144" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D144">
         <v>20</v>
@@ -6230,13 +6233,13 @@
     </row>
     <row r="145" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B145" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -6267,13 +6270,13 @@
     </row>
     <row r="146" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B146" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D146">
         <v>1</v>
@@ -6304,12 +6307,12 @@
     </row>
     <row r="147" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="148" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>16</v>
@@ -6346,7 +6349,7 @@
     </row>
     <row r="149" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>16</v>
@@ -6383,7 +6386,7 @@
     </row>
     <row r="150" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>16</v>
@@ -6419,7 +6422,7 @@
     </row>
     <row r="151" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>16</v>
@@ -6456,7 +6459,7 @@
     </row>
     <row r="152" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>16</v>
@@ -6493,7 +6496,7 @@
     </row>
     <row r="153" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B153" s="51" t="s">
         <v>16</v>
@@ -6530,7 +6533,7 @@
     </row>
     <row r="154" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B154" s="51" t="s">
         <v>16</v>
@@ -6539,35 +6542,35 @@
       <c r="I154"/>
       <c r="J154"/>
       <c r="L154" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="56" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B157" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B157" s="60" t="s">
+      <c r="C157" s="60" t="s">
         <v>63</v>
-      </c>
-      <c r="C157" s="60" t="s">
-        <v>64</v>
       </c>
       <c r="D157" s="57"/>
     </row>
     <row r="158" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="B158" s="61" t="s">
         <v>298</v>
       </c>
-      <c r="B158" s="61" t="s">
+      <c r="C158" s="61" t="s">
         <v>299</v>
-      </c>
-      <c r="C158" s="61" t="s">
-        <v>300</v>
       </c>
       <c r="D158" s="61"/>
       <c r="G158">
@@ -6576,11 +6579,11 @@
     </row>
     <row r="159" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="61" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B159" s="61"/>
       <c r="C159" s="61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D159" s="61"/>
       <c r="G159">
@@ -6589,11 +6592,11 @@
     </row>
     <row r="160" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B160" s="61"/>
       <c r="C160" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D160" s="61"/>
       <c r="G160">
@@ -6602,13 +6605,13 @@
     </row>
     <row r="161" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="B161" s="61" t="s">
         <v>305</v>
       </c>
-      <c r="B161" s="61" t="s">
+      <c r="C161" s="61" t="s">
         <v>306</v>
-      </c>
-      <c r="C161" s="61" t="s">
-        <v>307</v>
       </c>
       <c r="D161" s="61"/>
       <c r="G161">
@@ -6617,13 +6620,13 @@
     </row>
     <row r="162" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="61" t="s">
+        <v>307</v>
+      </c>
+      <c r="B162" s="61" t="s">
         <v>308</v>
       </c>
-      <c r="B162" s="61" t="s">
+      <c r="C162" s="61" t="s">
         <v>309</v>
-      </c>
-      <c r="C162" s="61" t="s">
-        <v>310</v>
       </c>
       <c r="D162" s="61"/>
       <c r="G162">
@@ -6632,13 +6635,13 @@
     </row>
     <row r="163" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B163" s="61" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C163" s="61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D163" s="61"/>
       <c r="G163">
@@ -6647,13 +6650,13 @@
     </row>
     <row r="164" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="61" t="s">
+        <v>311</v>
+      </c>
+      <c r="B164" s="61" t="s">
         <v>312</v>
       </c>
-      <c r="B164" s="61" t="s">
+      <c r="C164" s="61" t="s">
         <v>313</v>
-      </c>
-      <c r="C164" s="61" t="s">
-        <v>314</v>
       </c>
       <c r="D164" s="61"/>
       <c r="G164">
@@ -6662,13 +6665,13 @@
     </row>
     <row r="165" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="61" t="s">
+        <v>314</v>
+      </c>
+      <c r="B165" s="61" t="s">
         <v>315</v>
       </c>
-      <c r="B165" s="61" t="s">
+      <c r="C165" s="61" t="s">
         <v>316</v>
-      </c>
-      <c r="C165" s="61" t="s">
-        <v>317</v>
       </c>
       <c r="D165" s="61"/>
       <c r="G165">
@@ -6677,13 +6680,13 @@
     </row>
     <row r="166" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="B166" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="B166" s="61" t="s">
-        <v>319</v>
-      </c>
       <c r="C166" s="61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D166" s="61"/>
       <c r="G166">
@@ -6692,30 +6695,30 @@
     </row>
     <row r="167" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="56" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="168" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B168" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B168" s="60" t="s">
+      <c r="C168" s="60" t="s">
         <v>63</v>
-      </c>
-      <c r="C168" s="60" t="s">
-        <v>64</v>
       </c>
       <c r="D168" s="57"/>
     </row>
     <row r="169" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>320</v>
+      </c>
+      <c r="B169" t="s">
+        <v>308</v>
+      </c>
+      <c r="C169" t="s">
         <v>321</v>
-      </c>
-      <c r="B169" t="s">
-        <v>309</v>
-      </c>
-      <c r="C169" t="s">
-        <v>322</v>
       </c>
       <c r="G169">
         <v>2</v>
@@ -6723,13 +6726,13 @@
     </row>
     <row r="170" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
+        <v>322</v>
+      </c>
+      <c r="B170" t="s">
+        <v>90</v>
+      </c>
+      <c r="C170" t="s">
         <v>323</v>
-      </c>
-      <c r="B170" t="s">
-        <v>91</v>
-      </c>
-      <c r="C170" t="s">
-        <v>324</v>
       </c>
       <c r="G170">
         <v>3</v>
@@ -6737,13 +6740,13 @@
     </row>
     <row r="171" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
+        <v>324</v>
+      </c>
+      <c r="B171" t="s">
+        <v>90</v>
+      </c>
+      <c r="C171" t="s">
         <v>325</v>
-      </c>
-      <c r="B171" t="s">
-        <v>91</v>
-      </c>
-      <c r="C171" t="s">
-        <v>326</v>
       </c>
       <c r="G171">
         <v>4</v>
@@ -6751,13 +6754,13 @@
     </row>
     <row r="172" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
+        <v>326</v>
+      </c>
+      <c r="B172" t="s">
+        <v>90</v>
+      </c>
+      <c r="C172" t="s">
         <v>327</v>
-      </c>
-      <c r="B172" t="s">
-        <v>91</v>
-      </c>
-      <c r="C172" t="s">
-        <v>328</v>
       </c>
       <c r="G172">
         <v>5</v>
@@ -6765,7 +6768,7 @@
     </row>
     <row r="174" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="53" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B174" s="53"/>
       <c r="C174" s="53"/>
@@ -6779,12 +6782,12 @@
       <c r="K174" s="53"/>
       <c r="L174" s="53"/>
       <c r="M174" s="31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="175" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I175"/>
       <c r="J175"/>
@@ -6796,10 +6799,10 @@
     <row r="176" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="41"/>
       <c r="B176" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="C176" s="41" t="s">
         <v>332</v>
-      </c>
-      <c r="C176" s="41" t="s">
-        <v>333</v>
       </c>
       <c r="F176" s="41"/>
       <c r="I176"/>
@@ -6807,7 +6810,7 @@
     </row>
     <row r="177" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I177"/>
       <c r="J177"/>
@@ -6898,27 +6901,27 @@
     </row>
     <row r="184" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C184" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D184">
         <f>SUM(D178:D183)</f>
         <v>14.202000000000004</v>
       </c>
       <c r="E184" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I184"/>
       <c r="J184"/>
     </row>
     <row r="185" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C185" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D185">
         <v>0.06</v>
       </c>
       <c r="E185" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F185" s="42"/>
       <c r="I185"/>
@@ -6926,27 +6929,27 @@
     </row>
     <row r="186" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C186" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D186">
         <f>D185*D184</f>
         <v>0.85212000000000021</v>
       </c>
       <c r="E186" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F186" s="43">
         <v>95.787000000000006</v>
       </c>
       <c r="G186" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I186"/>
       <c r="J186"/>
     </row>
     <row r="187" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D187" s="45" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F187" s="46">
         <f>F186*D186</f>
@@ -6958,14 +6961,14 @@
     <row r="188" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C188" s="45"/>
       <c r="D188" s="47" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I188"/>
       <c r="J188"/>
     </row>
     <row r="189" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="37" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B189" s="37"/>
       <c r="C189" s="37"/>
@@ -6981,7 +6984,7 @@
       </c>
       <c r="G189" s="37"/>
       <c r="H189" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I189" s="37"/>
       <c r="J189" s="37"/>
@@ -7006,7 +7009,7 @@
     </row>
     <row r="191" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I191"/>
       <c r="J191"/>
@@ -7031,40 +7034,40 @@
     </row>
     <row r="194" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I194"/>
       <c r="J194"/>
     </row>
     <row r="195" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B195" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D195">
         <v>0.73</v>
       </c>
       <c r="E195" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I195"/>
       <c r="J195"/>
     </row>
     <row r="196" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B196" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D196">
         <v>2.33</v>
       </c>
       <c r="E196" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I196"/>
       <c r="J196"/>
     </row>
     <row r="197" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D197">
         <v>2</v>
@@ -7074,27 +7077,27 @@
     </row>
     <row r="198" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B198" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D198" s="45">
         <f>D195*D196*D197</f>
         <v>3.4018000000000002</v>
       </c>
       <c r="E198" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F198" s="47">
         <v>23.83</v>
       </c>
       <c r="G198" s="49" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I198"/>
       <c r="J198"/>
     </row>
     <row r="199" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D199" s="50" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E199" s="45"/>
       <c r="F199" s="46">
@@ -7110,10 +7113,10 @@
     </row>
     <row r="201" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>347</v>
+      </c>
+      <c r="H201" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="H201" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="I201"/>
       <c r="J201"/>
@@ -7124,17 +7127,17 @@
     </row>
     <row r="203" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I203"/>
       <c r="J203"/>
     </row>
     <row r="204" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B204" t="s">
+        <v>331</v>
+      </c>
+      <c r="C204" t="s">
         <v>332</v>
-      </c>
-      <c r="C204" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="205" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7153,15 +7156,15 @@
         <v>4</v>
       </c>
       <c r="G206" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="207" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D207" s="45" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F207" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="213" spans="14:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7528,15 +7531,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F27CC6-C2D0-4874-8769-D37D775F3894}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="4e601f28-1cb4-4d51-afb5-405c24b0aef5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="4e601f28-1cb4-4d51-afb5-405c24b0aef5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="7b5640c2-0ef9-45b5-a224-2dec6e355c8b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>